<commit_message>
Att todos os resultados
</commit_message>
<xml_diff>
--- a/VNL Masculino 2025.xlsx
+++ b/VNL Masculino 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1A96F3-118A-42DF-ADBF-EAC249FC1E55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E407639-59F5-4F8D-8D1A-9B1F431F2B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC01" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="2" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
@@ -921,39 +921,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -970,10 +937,43 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5378,16 +5378,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="S25:W25"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:W1"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="S25:W25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5456,88 +5456,88 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:64" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="AU2" s="79" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="90"/>
+      <c r="Y2" s="90"/>
+      <c r="AU2" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="80"/>
-      <c r="AW2" s="81"/>
-      <c r="AX2" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY2" s="80"/>
-      <c r="AZ2" s="81"/>
-      <c r="BA2" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB2" s="80"/>
-      <c r="BC2" s="80"/>
-      <c r="BD2" s="80"/>
-      <c r="BE2" s="80"/>
-      <c r="BF2" s="81"/>
-      <c r="BG2" s="79" t="s">
+      <c r="AV2" s="84"/>
+      <c r="AW2" s="85"/>
+      <c r="AX2" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="84"/>
+      <c r="AZ2" s="85"/>
+      <c r="BA2" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="84"/>
+      <c r="BC2" s="84"/>
+      <c r="BD2" s="84"/>
+      <c r="BE2" s="84"/>
+      <c r="BF2" s="85"/>
+      <c r="BG2" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="BH2" s="80"/>
-      <c r="BI2" s="81"/>
-      <c r="BJ2" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="BK2" s="80"/>
-      <c r="BL2" s="81"/>
+      <c r="BH2" s="84"/>
+      <c r="BI2" s="85"/>
+      <c r="BJ2" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK2" s="84"/>
+      <c r="BL2" s="85"/>
     </row>
     <row r="3" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="75"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
       <c r="AU3" s="32" t="s">
         <v>7</v>
       </c>
@@ -5598,42 +5598,42 @@
         <v>52</v>
       </c>
       <c r="C4" s="24"/>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="74" t="s">
+      <c r="H4" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74" t="s">
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74" t="s">
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74" t="s">
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74" t="s">
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74" t="s">
+      <c r="U4" s="88"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
       <c r="AA4" s="4" t="s">
         <v>59</v>
       </c>
@@ -8404,32 +8404,32 @@
       </c>
     </row>
     <row r="17" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="75"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="75"/>
-      <c r="V17" s="75"/>
-      <c r="W17" s="75"/>
-      <c r="X17" s="75"/>
-      <c r="Y17" s="75"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="86"/>
+      <c r="R17" s="86"/>
+      <c r="S17" s="86"/>
+      <c r="T17" s="86"/>
+      <c r="U17" s="86"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="86"/>
+      <c r="X17" s="86"/>
+      <c r="Y17" s="86"/>
       <c r="AU17" s="31">
         <v>14</v>
       </c>
@@ -8507,42 +8507,42 @@
         <v>52</v>
       </c>
       <c r="C18" s="24"/>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="74" t="s">
+      <c r="H18" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74" t="s">
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="74" t="s">
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74" t="s">
+      <c r="O18" s="88"/>
+      <c r="P18" s="88"/>
+      <c r="Q18" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R18" s="74"/>
-      <c r="S18" s="74"/>
-      <c r="T18" s="74" t="s">
+      <c r="R18" s="88"/>
+      <c r="S18" s="88"/>
+      <c r="T18" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74" t="s">
+      <c r="U18" s="88"/>
+      <c r="V18" s="88"/>
+      <c r="W18" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X18" s="74"/>
-      <c r="Y18" s="74"/>
+      <c r="X18" s="88"/>
+      <c r="Y18" s="88"/>
       <c r="AA18" s="4" t="s">
         <v>59</v>
       </c>
@@ -10694,78 +10694,78 @@
       </c>
     </row>
     <row r="31" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="75"/>
-      <c r="N31" s="75"/>
-      <c r="O31" s="75"/>
-      <c r="P31" s="75"/>
-      <c r="Q31" s="75"/>
-      <c r="R31" s="75"/>
-      <c r="S31" s="75"/>
-      <c r="T31" s="75"/>
-      <c r="U31" s="75"/>
-      <c r="V31" s="75"/>
-      <c r="W31" s="75"/>
-      <c r="X31" s="75"/>
-      <c r="Y31" s="75"/>
-      <c r="AU31" s="83" t="s">
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="86"/>
+      <c r="Q31" s="86"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
+      <c r="T31" s="86"/>
+      <c r="U31" s="86"/>
+      <c r="V31" s="86"/>
+      <c r="W31" s="86"/>
+      <c r="X31" s="86"/>
+      <c r="Y31" s="86"/>
+      <c r="AU31" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="AV31" s="84"/>
+      <c r="AV31" s="79"/>
     </row>
     <row r="32" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B32" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="24"/>
-      <c r="D32" s="78" t="s">
+      <c r="D32" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="74" t="s">
+      <c r="H32" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74" t="s">
+      <c r="I32" s="88"/>
+      <c r="J32" s="88"/>
+      <c r="K32" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74" t="s">
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74" t="s">
+      <c r="O32" s="88"/>
+      <c r="P32" s="88"/>
+      <c r="Q32" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
-      <c r="T32" s="74" t="s">
+      <c r="R32" s="88"/>
+      <c r="S32" s="88"/>
+      <c r="T32" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U32" s="74"/>
-      <c r="V32" s="74"/>
-      <c r="W32" s="74" t="s">
+      <c r="U32" s="88"/>
+      <c r="V32" s="88"/>
+      <c r="W32" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X32" s="74"/>
-      <c r="Y32" s="74"/>
+      <c r="X32" s="88"/>
+      <c r="Y32" s="88"/>
       <c r="AA32" s="4" t="s">
         <v>59</v>
       </c>
@@ -10823,10 +10823,10 @@
       <c r="AT32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AU32" s="89" t="s">
+      <c r="AU32" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="AV32" s="90"/>
+      <c r="AV32" s="81"/>
     </row>
     <row r="33" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B33" s="17">
@@ -10975,10 +10975,10 @@
         <f t="shared" ref="AT33:AT44" si="59">IF(D33&lt;F33,SUM(J33,M33,P33,S33,V33),SUM(H33,K33,N33,Q33,T33))</f>
         <v>97</v>
       </c>
-      <c r="AU33" s="85" t="s">
+      <c r="AU33" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="AV33" s="86"/>
+      <c r="AV33" s="75"/>
     </row>
     <row r="34" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B34" s="17">
@@ -11123,10 +11123,10 @@
         <f t="shared" si="59"/>
         <v>75</v>
       </c>
-      <c r="AU34" s="85" t="s">
+      <c r="AU34" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="AV34" s="86"/>
+      <c r="AV34" s="75"/>
     </row>
     <row r="35" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B35" s="17">
@@ -11275,10 +11275,10 @@
         <f t="shared" si="59"/>
         <v>87</v>
       </c>
-      <c r="AU35" s="85" t="s">
+      <c r="AU35" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="AV35" s="86"/>
+      <c r="AV35" s="75"/>
     </row>
     <row r="36" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B36" s="17">
@@ -11423,10 +11423,10 @@
         <f t="shared" si="59"/>
         <v>75</v>
       </c>
-      <c r="AU36" s="87" t="s">
+      <c r="AU36" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="AV36" s="88"/>
+      <c r="AV36" s="77"/>
     </row>
     <row r="37" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
@@ -12593,88 +12593,88 @@
       </c>
     </row>
     <row r="46" spans="2:64" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="76"/>
-      <c r="J46" s="76"/>
-      <c r="K46" s="76"/>
-      <c r="L46" s="76"/>
-      <c r="M46" s="76"/>
-      <c r="N46" s="76"/>
-      <c r="O46" s="76"/>
-      <c r="P46" s="76"/>
-      <c r="Q46" s="76"/>
-      <c r="R46" s="76"/>
-      <c r="S46" s="76"/>
-      <c r="T46" s="76"/>
-      <c r="U46" s="76"/>
-      <c r="V46" s="76"/>
-      <c r="W46" s="76"/>
-      <c r="X46" s="76"/>
-      <c r="Y46" s="76"/>
-      <c r="AU46" s="79" t="s">
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="90"/>
+      <c r="N46" s="90"/>
+      <c r="O46" s="90"/>
+      <c r="P46" s="90"/>
+      <c r="Q46" s="90"/>
+      <c r="R46" s="90"/>
+      <c r="S46" s="90"/>
+      <c r="T46" s="90"/>
+      <c r="U46" s="90"/>
+      <c r="V46" s="90"/>
+      <c r="W46" s="90"/>
+      <c r="X46" s="90"/>
+      <c r="Y46" s="90"/>
+      <c r="AU46" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="AV46" s="80"/>
-      <c r="AW46" s="81"/>
-      <c r="AX46" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY46" s="80"/>
-      <c r="AZ46" s="81"/>
-      <c r="BA46" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB46" s="80"/>
-      <c r="BC46" s="80"/>
-      <c r="BD46" s="80"/>
-      <c r="BE46" s="80"/>
-      <c r="BF46" s="81"/>
-      <c r="BG46" s="79" t="s">
+      <c r="AV46" s="84"/>
+      <c r="AW46" s="85"/>
+      <c r="AX46" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY46" s="84"/>
+      <c r="AZ46" s="85"/>
+      <c r="BA46" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB46" s="84"/>
+      <c r="BC46" s="84"/>
+      <c r="BD46" s="84"/>
+      <c r="BE46" s="84"/>
+      <c r="BF46" s="85"/>
+      <c r="BG46" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="BH46" s="80"/>
-      <c r="BI46" s="81"/>
-      <c r="BJ46" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="BK46" s="80"/>
-      <c r="BL46" s="81"/>
+      <c r="BH46" s="84"/>
+      <c r="BI46" s="85"/>
+      <c r="BJ46" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK46" s="84"/>
+      <c r="BL46" s="85"/>
     </row>
     <row r="47" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="75" t="s">
+      <c r="B47" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="75"/>
-      <c r="L47" s="75"/>
-      <c r="M47" s="75"/>
-      <c r="N47" s="75"/>
-      <c r="O47" s="75"/>
-      <c r="P47" s="75"/>
-      <c r="Q47" s="75"/>
-      <c r="R47" s="75"/>
-      <c r="S47" s="75"/>
-      <c r="T47" s="75"/>
-      <c r="U47" s="75"/>
-      <c r="V47" s="75"/>
-      <c r="W47" s="75"/>
-      <c r="X47" s="75"/>
-      <c r="Y47" s="75"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86"/>
+      <c r="H47" s="86"/>
+      <c r="I47" s="86"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+      <c r="N47" s="86"/>
+      <c r="O47" s="86"/>
+      <c r="P47" s="86"/>
+      <c r="Q47" s="86"/>
+      <c r="R47" s="86"/>
+      <c r="S47" s="86"/>
+      <c r="T47" s="86"/>
+      <c r="U47" s="86"/>
+      <c r="V47" s="86"/>
+      <c r="W47" s="86"/>
+      <c r="X47" s="86"/>
+      <c r="Y47" s="86"/>
       <c r="AU47" s="32" t="s">
         <v>7</v>
       </c>
@@ -12735,42 +12735,42 @@
         <v>52</v>
       </c>
       <c r="C48" s="24"/>
-      <c r="D48" s="78" t="s">
+      <c r="D48" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="87"/>
       <c r="G48" s="20"/>
-      <c r="H48" s="74" t="s">
+      <c r="H48" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I48" s="74"/>
-      <c r="J48" s="74"/>
-      <c r="K48" s="74" t="s">
+      <c r="I48" s="88"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L48" s="74"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="74" t="s">
+      <c r="L48" s="88"/>
+      <c r="M48" s="88"/>
+      <c r="N48" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O48" s="74"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="74" t="s">
+      <c r="O48" s="88"/>
+      <c r="P48" s="88"/>
+      <c r="Q48" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R48" s="74"/>
-      <c r="S48" s="74"/>
-      <c r="T48" s="74" t="s">
+      <c r="R48" s="88"/>
+      <c r="S48" s="88"/>
+      <c r="T48" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U48" s="74"/>
-      <c r="V48" s="74"/>
-      <c r="W48" s="74" t="s">
+      <c r="U48" s="88"/>
+      <c r="V48" s="88"/>
+      <c r="W48" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X48" s="74"/>
-      <c r="Y48" s="74"/>
+      <c r="X48" s="88"/>
+      <c r="Y48" s="88"/>
       <c r="AA48" s="4" t="s">
         <v>59</v>
       </c>
@@ -15505,32 +15505,32 @@
       </c>
     </row>
     <row r="61" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="75" t="s">
+      <c r="B61" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="75"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="77"/>
-      <c r="F61" s="75"/>
-      <c r="G61" s="75"/>
-      <c r="H61" s="75"/>
-      <c r="I61" s="75"/>
-      <c r="J61" s="75"/>
-      <c r="K61" s="75"/>
-      <c r="L61" s="75"/>
-      <c r="M61" s="75"/>
-      <c r="N61" s="75"/>
-      <c r="O61" s="75"/>
-      <c r="P61" s="75"/>
-      <c r="Q61" s="75"/>
-      <c r="R61" s="75"/>
-      <c r="S61" s="75"/>
-      <c r="T61" s="75"/>
-      <c r="U61" s="75"/>
-      <c r="V61" s="75"/>
-      <c r="W61" s="75"/>
-      <c r="X61" s="75"/>
-      <c r="Y61" s="75"/>
+      <c r="C61" s="86"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="86"/>
+      <c r="G61" s="86"/>
+      <c r="H61" s="86"/>
+      <c r="I61" s="86"/>
+      <c r="J61" s="86"/>
+      <c r="K61" s="86"/>
+      <c r="L61" s="86"/>
+      <c r="M61" s="86"/>
+      <c r="N61" s="86"/>
+      <c r="O61" s="86"/>
+      <c r="P61" s="86"/>
+      <c r="Q61" s="86"/>
+      <c r="R61" s="86"/>
+      <c r="S61" s="86"/>
+      <c r="T61" s="86"/>
+      <c r="U61" s="86"/>
+      <c r="V61" s="86"/>
+      <c r="W61" s="86"/>
+      <c r="X61" s="86"/>
+      <c r="Y61" s="86"/>
       <c r="AU61" s="31">
         <v>14</v>
       </c>
@@ -15608,42 +15608,42 @@
         <v>52</v>
       </c>
       <c r="C62" s="24"/>
-      <c r="D62" s="74" t="s">
+      <c r="D62" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
+      <c r="E62" s="88"/>
+      <c r="F62" s="88"/>
       <c r="G62" s="20"/>
-      <c r="H62" s="74" t="s">
+      <c r="H62" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I62" s="74"/>
-      <c r="J62" s="74"/>
-      <c r="K62" s="74" t="s">
+      <c r="I62" s="88"/>
+      <c r="J62" s="88"/>
+      <c r="K62" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L62" s="74"/>
-      <c r="M62" s="74"/>
-      <c r="N62" s="74" t="s">
+      <c r="L62" s="88"/>
+      <c r="M62" s="88"/>
+      <c r="N62" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O62" s="74"/>
-      <c r="P62" s="74"/>
-      <c r="Q62" s="74" t="s">
+      <c r="O62" s="88"/>
+      <c r="P62" s="88"/>
+      <c r="Q62" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R62" s="74"/>
-      <c r="S62" s="74"/>
-      <c r="T62" s="74" t="s">
+      <c r="R62" s="88"/>
+      <c r="S62" s="88"/>
+      <c r="T62" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U62" s="74"/>
-      <c r="V62" s="74"/>
-      <c r="W62" s="74" t="s">
+      <c r="U62" s="88"/>
+      <c r="V62" s="88"/>
+      <c r="W62" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X62" s="74"/>
-      <c r="Y62" s="74"/>
+      <c r="X62" s="88"/>
+      <c r="Y62" s="88"/>
       <c r="AA62" s="4" t="s">
         <v>59</v>
       </c>
@@ -17771,78 +17771,78 @@
       </c>
     </row>
     <row r="75" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="75" t="s">
+      <c r="B75" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="C75" s="75"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="75"/>
-      <c r="K75" s="75"/>
-      <c r="L75" s="75"/>
-      <c r="M75" s="75"/>
-      <c r="N75" s="75"/>
-      <c r="O75" s="75"/>
-      <c r="P75" s="75"/>
-      <c r="Q75" s="75"/>
-      <c r="R75" s="75"/>
-      <c r="S75" s="75"/>
-      <c r="T75" s="75"/>
-      <c r="U75" s="75"/>
-      <c r="V75" s="75"/>
-      <c r="W75" s="75"/>
-      <c r="X75" s="75"/>
-      <c r="Y75" s="75"/>
-      <c r="AU75" s="83" t="s">
+      <c r="C75" s="86"/>
+      <c r="D75" s="86"/>
+      <c r="E75" s="86"/>
+      <c r="F75" s="86"/>
+      <c r="G75" s="86"/>
+      <c r="H75" s="86"/>
+      <c r="I75" s="86"/>
+      <c r="J75" s="86"/>
+      <c r="K75" s="86"/>
+      <c r="L75" s="86"/>
+      <c r="M75" s="86"/>
+      <c r="N75" s="86"/>
+      <c r="O75" s="86"/>
+      <c r="P75" s="86"/>
+      <c r="Q75" s="86"/>
+      <c r="R75" s="86"/>
+      <c r="S75" s="86"/>
+      <c r="T75" s="86"/>
+      <c r="U75" s="86"/>
+      <c r="V75" s="86"/>
+      <c r="W75" s="86"/>
+      <c r="X75" s="86"/>
+      <c r="Y75" s="86"/>
+      <c r="AU75" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="AV75" s="84"/>
+      <c r="AV75" s="79"/>
     </row>
     <row r="76" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C76" s="24"/>
-      <c r="D76" s="78" t="s">
+      <c r="D76" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E76" s="78"/>
-      <c r="F76" s="78"/>
+      <c r="E76" s="87"/>
+      <c r="F76" s="87"/>
       <c r="G76" s="20"/>
-      <c r="H76" s="74" t="s">
+      <c r="H76" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I76" s="74"/>
-      <c r="J76" s="74"/>
-      <c r="K76" s="74" t="s">
+      <c r="I76" s="88"/>
+      <c r="J76" s="88"/>
+      <c r="K76" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L76" s="74"/>
-      <c r="M76" s="74"/>
-      <c r="N76" s="74" t="s">
+      <c r="L76" s="88"/>
+      <c r="M76" s="88"/>
+      <c r="N76" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O76" s="74"/>
-      <c r="P76" s="74"/>
-      <c r="Q76" s="74" t="s">
+      <c r="O76" s="88"/>
+      <c r="P76" s="88"/>
+      <c r="Q76" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R76" s="74"/>
-      <c r="S76" s="74"/>
-      <c r="T76" s="74" t="s">
+      <c r="R76" s="88"/>
+      <c r="S76" s="88"/>
+      <c r="T76" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U76" s="74"/>
-      <c r="V76" s="74"/>
-      <c r="W76" s="74" t="s">
+      <c r="U76" s="88"/>
+      <c r="V76" s="88"/>
+      <c r="W76" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X76" s="74"/>
-      <c r="Y76" s="74"/>
+      <c r="X76" s="88"/>
+      <c r="Y76" s="88"/>
       <c r="AA76" s="4" t="s">
         <v>59</v>
       </c>
@@ -17900,10 +17900,10 @@
       <c r="AT76" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AU76" s="89" t="s">
+      <c r="AU76" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="AV76" s="90"/>
+      <c r="AV76" s="81"/>
     </row>
     <row r="77" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B77" s="17">
@@ -18052,10 +18052,10 @@
         <f t="shared" ref="AT77:AT88" si="122">IF(D77&lt;F77,SUM(J77,M77,P77,S77,V77),SUM(H77,K77,N77,Q77,T77))</f>
         <v>94</v>
       </c>
-      <c r="AU77" s="85" t="s">
+      <c r="AU77" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="AV77" s="86"/>
+      <c r="AV77" s="75"/>
     </row>
     <row r="78" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B78" s="17">
@@ -18200,10 +18200,10 @@
         <f t="shared" si="122"/>
         <v>75</v>
       </c>
-      <c r="AU78" s="85" t="s">
+      <c r="AU78" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="AV78" s="86"/>
+      <c r="AV78" s="75"/>
     </row>
     <row r="79" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B79" s="17">
@@ -18352,10 +18352,10 @@
         <f t="shared" si="122"/>
         <v>98</v>
       </c>
-      <c r="AU79" s="85" t="s">
+      <c r="AU79" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="AV79" s="86"/>
+      <c r="AV79" s="75"/>
     </row>
     <row r="80" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B80" s="17">
@@ -18504,10 +18504,10 @@
         <f t="shared" si="122"/>
         <v>100</v>
       </c>
-      <c r="AU80" s="87" t="s">
+      <c r="AU80" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="AV80" s="88"/>
+      <c r="AV80" s="77"/>
     </row>
     <row r="81" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B81" s="17">
@@ -19702,88 +19702,88 @@
       </c>
     </row>
     <row r="90" spans="2:64" ht="15" x14ac:dyDescent="0.25">
-      <c r="B90" s="76" t="s">
+      <c r="B90" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="C90" s="76"/>
-      <c r="D90" s="76"/>
-      <c r="E90" s="76"/>
-      <c r="F90" s="76"/>
-      <c r="G90" s="76"/>
-      <c r="H90" s="76"/>
-      <c r="I90" s="76"/>
-      <c r="J90" s="76"/>
-      <c r="K90" s="76"/>
-      <c r="L90" s="76"/>
-      <c r="M90" s="76"/>
-      <c r="N90" s="76"/>
-      <c r="O90" s="76"/>
-      <c r="P90" s="76"/>
-      <c r="Q90" s="76"/>
-      <c r="R90" s="76"/>
-      <c r="S90" s="76"/>
-      <c r="T90" s="76"/>
-      <c r="U90" s="76"/>
-      <c r="V90" s="76"/>
-      <c r="W90" s="76"/>
-      <c r="X90" s="76"/>
-      <c r="Y90" s="76"/>
-      <c r="AU90" s="79" t="s">
+      <c r="C90" s="90"/>
+      <c r="D90" s="90"/>
+      <c r="E90" s="90"/>
+      <c r="F90" s="90"/>
+      <c r="G90" s="90"/>
+      <c r="H90" s="90"/>
+      <c r="I90" s="90"/>
+      <c r="J90" s="90"/>
+      <c r="K90" s="90"/>
+      <c r="L90" s="90"/>
+      <c r="M90" s="90"/>
+      <c r="N90" s="90"/>
+      <c r="O90" s="90"/>
+      <c r="P90" s="90"/>
+      <c r="Q90" s="90"/>
+      <c r="R90" s="90"/>
+      <c r="S90" s="90"/>
+      <c r="T90" s="90"/>
+      <c r="U90" s="90"/>
+      <c r="V90" s="90"/>
+      <c r="W90" s="90"/>
+      <c r="X90" s="90"/>
+      <c r="Y90" s="90"/>
+      <c r="AU90" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="AV90" s="80"/>
-      <c r="AW90" s="81"/>
-      <c r="AX90" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY90" s="80"/>
-      <c r="AZ90" s="81"/>
-      <c r="BA90" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB90" s="80"/>
-      <c r="BC90" s="80"/>
-      <c r="BD90" s="80"/>
-      <c r="BE90" s="80"/>
-      <c r="BF90" s="81"/>
-      <c r="BG90" s="79" t="s">
+      <c r="AV90" s="84"/>
+      <c r="AW90" s="85"/>
+      <c r="AX90" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY90" s="84"/>
+      <c r="AZ90" s="85"/>
+      <c r="BA90" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB90" s="84"/>
+      <c r="BC90" s="84"/>
+      <c r="BD90" s="84"/>
+      <c r="BE90" s="84"/>
+      <c r="BF90" s="85"/>
+      <c r="BG90" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="BH90" s="80"/>
-      <c r="BI90" s="81"/>
-      <c r="BJ90" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="BK90" s="80"/>
-      <c r="BL90" s="81"/>
+      <c r="BH90" s="84"/>
+      <c r="BI90" s="85"/>
+      <c r="BJ90" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK90" s="84"/>
+      <c r="BL90" s="85"/>
     </row>
     <row r="91" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B91" s="75" t="s">
+      <c r="B91" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="C91" s="75"/>
-      <c r="D91" s="75"/>
-      <c r="E91" s="75"/>
-      <c r="F91" s="75"/>
-      <c r="G91" s="75"/>
-      <c r="H91" s="75"/>
-      <c r="I91" s="75"/>
-      <c r="J91" s="75"/>
-      <c r="K91" s="75"/>
-      <c r="L91" s="75"/>
-      <c r="M91" s="75"/>
-      <c r="N91" s="75"/>
-      <c r="O91" s="75"/>
-      <c r="P91" s="75"/>
-      <c r="Q91" s="75"/>
-      <c r="R91" s="75"/>
-      <c r="S91" s="75"/>
-      <c r="T91" s="75"/>
-      <c r="U91" s="75"/>
-      <c r="V91" s="75"/>
-      <c r="W91" s="75"/>
-      <c r="X91" s="75"/>
-      <c r="Y91" s="75"/>
+      <c r="C91" s="86"/>
+      <c r="D91" s="86"/>
+      <c r="E91" s="86"/>
+      <c r="F91" s="86"/>
+      <c r="G91" s="86"/>
+      <c r="H91" s="86"/>
+      <c r="I91" s="86"/>
+      <c r="J91" s="86"/>
+      <c r="K91" s="86"/>
+      <c r="L91" s="86"/>
+      <c r="M91" s="86"/>
+      <c r="N91" s="86"/>
+      <c r="O91" s="86"/>
+      <c r="P91" s="86"/>
+      <c r="Q91" s="86"/>
+      <c r="R91" s="86"/>
+      <c r="S91" s="86"/>
+      <c r="T91" s="86"/>
+      <c r="U91" s="86"/>
+      <c r="V91" s="86"/>
+      <c r="W91" s="86"/>
+      <c r="X91" s="86"/>
+      <c r="Y91" s="86"/>
       <c r="AU91" s="32" t="s">
         <v>7</v>
       </c>
@@ -19844,42 +19844,42 @@
         <v>52</v>
       </c>
       <c r="C92" s="24"/>
-      <c r="D92" s="78" t="s">
+      <c r="D92" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E92" s="78"/>
-      <c r="F92" s="78"/>
+      <c r="E92" s="87"/>
+      <c r="F92" s="87"/>
       <c r="G92" s="20"/>
-      <c r="H92" s="74" t="s">
+      <c r="H92" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I92" s="74"/>
-      <c r="J92" s="74"/>
-      <c r="K92" s="74" t="s">
+      <c r="I92" s="88"/>
+      <c r="J92" s="88"/>
+      <c r="K92" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L92" s="74"/>
-      <c r="M92" s="74"/>
-      <c r="N92" s="74" t="s">
+      <c r="L92" s="88"/>
+      <c r="M92" s="88"/>
+      <c r="N92" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O92" s="74"/>
-      <c r="P92" s="74"/>
-      <c r="Q92" s="74" t="s">
+      <c r="O92" s="88"/>
+      <c r="P92" s="88"/>
+      <c r="Q92" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R92" s="74"/>
-      <c r="S92" s="74"/>
-      <c r="T92" s="74" t="s">
+      <c r="R92" s="88"/>
+      <c r="S92" s="88"/>
+      <c r="T92" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U92" s="74"/>
-      <c r="V92" s="74"/>
-      <c r="W92" s="74" t="s">
+      <c r="U92" s="88"/>
+      <c r="V92" s="88"/>
+      <c r="W92" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X92" s="74"/>
-      <c r="Y92" s="74"/>
+      <c r="X92" s="88"/>
+      <c r="Y92" s="88"/>
       <c r="AA92" s="4" t="s">
         <v>59</v>
       </c>
@@ -22646,32 +22646,32 @@
       </c>
     </row>
     <row r="105" spans="2:64" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B105" s="75" t="s">
+      <c r="B105" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="C105" s="75"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="77"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="75"/>
-      <c r="H105" s="75"/>
-      <c r="I105" s="75"/>
-      <c r="J105" s="75"/>
-      <c r="K105" s="75"/>
-      <c r="L105" s="75"/>
-      <c r="M105" s="75"/>
-      <c r="N105" s="75"/>
-      <c r="O105" s="75"/>
-      <c r="P105" s="75"/>
-      <c r="Q105" s="75"/>
-      <c r="R105" s="75"/>
-      <c r="S105" s="75"/>
-      <c r="T105" s="75"/>
-      <c r="U105" s="75"/>
-      <c r="V105" s="75"/>
-      <c r="W105" s="75"/>
-      <c r="X105" s="75"/>
-      <c r="Y105" s="75"/>
+      <c r="C105" s="86"/>
+      <c r="D105" s="86"/>
+      <c r="E105" s="89"/>
+      <c r="F105" s="86"/>
+      <c r="G105" s="86"/>
+      <c r="H105" s="86"/>
+      <c r="I105" s="86"/>
+      <c r="J105" s="86"/>
+      <c r="K105" s="86"/>
+      <c r="L105" s="86"/>
+      <c r="M105" s="86"/>
+      <c r="N105" s="86"/>
+      <c r="O105" s="86"/>
+      <c r="P105" s="86"/>
+      <c r="Q105" s="86"/>
+      <c r="R105" s="86"/>
+      <c r="S105" s="86"/>
+      <c r="T105" s="86"/>
+      <c r="U105" s="86"/>
+      <c r="V105" s="86"/>
+      <c r="W105" s="86"/>
+      <c r="X105" s="86"/>
+      <c r="Y105" s="86"/>
       <c r="AU105" s="31">
         <v>14</v>
       </c>
@@ -22749,42 +22749,42 @@
         <v>52</v>
       </c>
       <c r="C106" s="24"/>
-      <c r="D106" s="74" t="s">
+      <c r="D106" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
+      <c r="E106" s="88"/>
+      <c r="F106" s="88"/>
       <c r="G106" s="20"/>
-      <c r="H106" s="74" t="s">
+      <c r="H106" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I106" s="74"/>
-      <c r="J106" s="74"/>
-      <c r="K106" s="74" t="s">
+      <c r="I106" s="88"/>
+      <c r="J106" s="88"/>
+      <c r="K106" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L106" s="74"/>
-      <c r="M106" s="74"/>
-      <c r="N106" s="74" t="s">
+      <c r="L106" s="88"/>
+      <c r="M106" s="88"/>
+      <c r="N106" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O106" s="74"/>
-      <c r="P106" s="74"/>
-      <c r="Q106" s="74" t="s">
+      <c r="O106" s="88"/>
+      <c r="P106" s="88"/>
+      <c r="Q106" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R106" s="74"/>
-      <c r="S106" s="74"/>
-      <c r="T106" s="74" t="s">
+      <c r="R106" s="88"/>
+      <c r="S106" s="88"/>
+      <c r="T106" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U106" s="74"/>
-      <c r="V106" s="74"/>
-      <c r="W106" s="74" t="s">
+      <c r="U106" s="88"/>
+      <c r="V106" s="88"/>
+      <c r="W106" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X106" s="74"/>
-      <c r="Y106" s="74"/>
+      <c r="X106" s="88"/>
+      <c r="Y106" s="88"/>
       <c r="AA106" s="4" t="s">
         <v>59</v>
       </c>
@@ -24912,78 +24912,78 @@
       </c>
     </row>
     <row r="119" spans="2:48" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B119" s="75" t="s">
+      <c r="B119" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="C119" s="75"/>
-      <c r="D119" s="75"/>
-      <c r="E119" s="75"/>
-      <c r="F119" s="75"/>
-      <c r="G119" s="75"/>
-      <c r="H119" s="75"/>
-      <c r="I119" s="75"/>
-      <c r="J119" s="75"/>
-      <c r="K119" s="75"/>
-      <c r="L119" s="75"/>
-      <c r="M119" s="75"/>
-      <c r="N119" s="75"/>
-      <c r="O119" s="75"/>
-      <c r="P119" s="75"/>
-      <c r="Q119" s="75"/>
-      <c r="R119" s="75"/>
-      <c r="S119" s="75"/>
-      <c r="T119" s="75"/>
-      <c r="U119" s="75"/>
-      <c r="V119" s="75"/>
-      <c r="W119" s="75"/>
-      <c r="X119" s="75"/>
-      <c r="Y119" s="75"/>
-      <c r="AU119" s="83" t="s">
+      <c r="C119" s="86"/>
+      <c r="D119" s="86"/>
+      <c r="E119" s="86"/>
+      <c r="F119" s="86"/>
+      <c r="G119" s="86"/>
+      <c r="H119" s="86"/>
+      <c r="I119" s="86"/>
+      <c r="J119" s="86"/>
+      <c r="K119" s="86"/>
+      <c r="L119" s="86"/>
+      <c r="M119" s="86"/>
+      <c r="N119" s="86"/>
+      <c r="O119" s="86"/>
+      <c r="P119" s="86"/>
+      <c r="Q119" s="86"/>
+      <c r="R119" s="86"/>
+      <c r="S119" s="86"/>
+      <c r="T119" s="86"/>
+      <c r="U119" s="86"/>
+      <c r="V119" s="86"/>
+      <c r="W119" s="86"/>
+      <c r="X119" s="86"/>
+      <c r="Y119" s="86"/>
+      <c r="AU119" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="AV119" s="84"/>
+      <c r="AV119" s="79"/>
     </row>
     <row r="120" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B120" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C120" s="24"/>
-      <c r="D120" s="78" t="s">
+      <c r="D120" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E120" s="78"/>
-      <c r="F120" s="78"/>
+      <c r="E120" s="87"/>
+      <c r="F120" s="87"/>
       <c r="G120" s="20"/>
-      <c r="H120" s="74" t="s">
+      <c r="H120" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I120" s="74"/>
-      <c r="J120" s="74"/>
-      <c r="K120" s="74" t="s">
+      <c r="I120" s="88"/>
+      <c r="J120" s="88"/>
+      <c r="K120" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L120" s="74"/>
-      <c r="M120" s="74"/>
-      <c r="N120" s="74" t="s">
+      <c r="L120" s="88"/>
+      <c r="M120" s="88"/>
+      <c r="N120" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O120" s="74"/>
-      <c r="P120" s="74"/>
-      <c r="Q120" s="74" t="s">
+      <c r="O120" s="88"/>
+      <c r="P120" s="88"/>
+      <c r="Q120" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R120" s="74"/>
-      <c r="S120" s="74"/>
-      <c r="T120" s="74" t="s">
+      <c r="R120" s="88"/>
+      <c r="S120" s="88"/>
+      <c r="T120" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U120" s="74"/>
-      <c r="V120" s="74"/>
-      <c r="W120" s="74" t="s">
+      <c r="U120" s="88"/>
+      <c r="V120" s="88"/>
+      <c r="W120" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X120" s="74"/>
-      <c r="Y120" s="74"/>
+      <c r="X120" s="88"/>
+      <c r="Y120" s="88"/>
       <c r="AA120" s="4" t="s">
         <v>59</v>
       </c>
@@ -25041,10 +25041,10 @@
       <c r="AT120" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AU120" s="89" t="s">
+      <c r="AU120" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="AV120" s="90"/>
+      <c r="AV120" s="81"/>
     </row>
     <row r="121" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B121" s="17">
@@ -25189,10 +25189,10 @@
         <f t="shared" ref="AT121:AT132" si="185">IF(D121&lt;F121,SUM(J121,M121,P121,S121,V121),SUM(H121,K121,N121,Q121,T121))</f>
         <v>75</v>
       </c>
-      <c r="AU121" s="85" t="s">
+      <c r="AU121" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="AV121" s="86"/>
+      <c r="AV121" s="75"/>
     </row>
     <row r="122" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B122" s="17">
@@ -25341,10 +25341,10 @@
         <f t="shared" si="185"/>
         <v>99</v>
       </c>
-      <c r="AU122" s="85" t="s">
+      <c r="AU122" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="AV122" s="86"/>
+      <c r="AV122" s="75"/>
     </row>
     <row r="123" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B123" s="17">
@@ -25489,10 +25489,10 @@
         <f t="shared" si="185"/>
         <v>80</v>
       </c>
-      <c r="AU123" s="85" t="s">
+      <c r="AU123" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="AV123" s="86"/>
+      <c r="AV123" s="75"/>
     </row>
     <row r="124" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B124" s="17">
@@ -25641,10 +25641,10 @@
         <f t="shared" si="185"/>
         <v>96</v>
       </c>
-      <c r="AU124" s="87" t="s">
+      <c r="AU124" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="AV124" s="88"/>
+      <c r="AV124" s="77"/>
     </row>
     <row r="125" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B125" s="17">
@@ -26841,83 +26841,16 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="111">
-    <mergeCell ref="AU123:AV123"/>
-    <mergeCell ref="AU124:AV124"/>
-    <mergeCell ref="AU36:AV36"/>
-    <mergeCell ref="AU119:AV119"/>
-    <mergeCell ref="AU120:AV120"/>
-    <mergeCell ref="AU121:AV121"/>
-    <mergeCell ref="AU122:AV122"/>
-    <mergeCell ref="AU31:AV31"/>
-    <mergeCell ref="AU32:AV32"/>
-    <mergeCell ref="AU33:AV33"/>
-    <mergeCell ref="AU34:AV34"/>
-    <mergeCell ref="AU35:AV35"/>
-    <mergeCell ref="AU76:AV76"/>
-    <mergeCell ref="AU77:AV77"/>
-    <mergeCell ref="AU78:AV78"/>
-    <mergeCell ref="AU79:AV79"/>
-    <mergeCell ref="AU80:AV80"/>
-    <mergeCell ref="AU111:AV111"/>
-    <mergeCell ref="AU90:AW90"/>
-    <mergeCell ref="AX90:AZ90"/>
-    <mergeCell ref="BA90:BF90"/>
-    <mergeCell ref="BG90:BI90"/>
-    <mergeCell ref="BJ90:BL90"/>
-    <mergeCell ref="AU23:AV23"/>
-    <mergeCell ref="AU67:AV67"/>
-    <mergeCell ref="AX2:AZ2"/>
-    <mergeCell ref="BA2:BF2"/>
-    <mergeCell ref="BG2:BI2"/>
-    <mergeCell ref="BJ2:BL2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AU46:AW46"/>
-    <mergeCell ref="AX46:AZ46"/>
-    <mergeCell ref="BA46:BF46"/>
-    <mergeCell ref="BG46:BI46"/>
-    <mergeCell ref="BJ46:BL46"/>
-    <mergeCell ref="AU75:AV75"/>
-    <mergeCell ref="B119:Y119"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="H120:J120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="N120:P120"/>
-    <mergeCell ref="Q120:S120"/>
-    <mergeCell ref="T120:V120"/>
-    <mergeCell ref="W120:Y120"/>
-    <mergeCell ref="B105:Y105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="H106:J106"/>
-    <mergeCell ref="K106:M106"/>
-    <mergeCell ref="N106:P106"/>
-    <mergeCell ref="Q106:S106"/>
-    <mergeCell ref="T106:V106"/>
-    <mergeCell ref="W106:Y106"/>
-    <mergeCell ref="W76:Y76"/>
-    <mergeCell ref="B90:Y90"/>
-    <mergeCell ref="B91:Y91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:P92"/>
-    <mergeCell ref="Q92:S92"/>
-    <mergeCell ref="T92:V92"/>
-    <mergeCell ref="W92:Y92"/>
-    <mergeCell ref="D76:F76"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="K76:M76"/>
-    <mergeCell ref="N76:P76"/>
-    <mergeCell ref="Q76:S76"/>
-    <mergeCell ref="T76:V76"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="T62:V62"/>
-    <mergeCell ref="W62:Y62"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="N48:P48"/>
-    <mergeCell ref="Q48:S48"/>
-    <mergeCell ref="T48:V48"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="B3:Y3"/>
+    <mergeCell ref="B2:Y2"/>
+    <mergeCell ref="B17:Y17"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:V4"/>
     <mergeCell ref="B75:Y75"/>
     <mergeCell ref="B46:Y46"/>
     <mergeCell ref="B47:Y47"/>
@@ -26942,16 +26875,83 @@
     <mergeCell ref="H62:J62"/>
     <mergeCell ref="K62:M62"/>
     <mergeCell ref="N62:P62"/>
-    <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="B3:Y3"/>
-    <mergeCell ref="B2:Y2"/>
-    <mergeCell ref="B17:Y17"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="T62:V62"/>
+    <mergeCell ref="W62:Y62"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="N48:P48"/>
+    <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="T48:V48"/>
+    <mergeCell ref="W76:Y76"/>
+    <mergeCell ref="B90:Y90"/>
+    <mergeCell ref="B91:Y91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:P92"/>
+    <mergeCell ref="Q92:S92"/>
+    <mergeCell ref="T92:V92"/>
+    <mergeCell ref="W92:Y92"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="H76:J76"/>
+    <mergeCell ref="K76:M76"/>
+    <mergeCell ref="N76:P76"/>
+    <mergeCell ref="Q76:S76"/>
+    <mergeCell ref="T76:V76"/>
+    <mergeCell ref="B119:Y119"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="H120:J120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="N120:P120"/>
+    <mergeCell ref="Q120:S120"/>
+    <mergeCell ref="T120:V120"/>
+    <mergeCell ref="W120:Y120"/>
+    <mergeCell ref="B105:Y105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="H106:J106"/>
+    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="N106:P106"/>
+    <mergeCell ref="Q106:S106"/>
+    <mergeCell ref="T106:V106"/>
+    <mergeCell ref="W106:Y106"/>
+    <mergeCell ref="AX90:AZ90"/>
+    <mergeCell ref="BA90:BF90"/>
+    <mergeCell ref="BG90:BI90"/>
+    <mergeCell ref="BJ90:BL90"/>
+    <mergeCell ref="AU23:AV23"/>
+    <mergeCell ref="AU67:AV67"/>
+    <mergeCell ref="AX2:AZ2"/>
+    <mergeCell ref="BA2:BF2"/>
+    <mergeCell ref="BG2:BI2"/>
+    <mergeCell ref="BJ2:BL2"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AU46:AW46"/>
+    <mergeCell ref="AX46:AZ46"/>
+    <mergeCell ref="BA46:BF46"/>
+    <mergeCell ref="BG46:BI46"/>
+    <mergeCell ref="BJ46:BL46"/>
+    <mergeCell ref="AU75:AV75"/>
+    <mergeCell ref="AU123:AV123"/>
+    <mergeCell ref="AU124:AV124"/>
+    <mergeCell ref="AU36:AV36"/>
+    <mergeCell ref="AU119:AV119"/>
+    <mergeCell ref="AU120:AV120"/>
+    <mergeCell ref="AU121:AV121"/>
+    <mergeCell ref="AU122:AV122"/>
+    <mergeCell ref="AU31:AV31"/>
+    <mergeCell ref="AU32:AV32"/>
+    <mergeCell ref="AU33:AV33"/>
+    <mergeCell ref="AU34:AV34"/>
+    <mergeCell ref="AU35:AV35"/>
+    <mergeCell ref="AU76:AV76"/>
+    <mergeCell ref="AU77:AV77"/>
+    <mergeCell ref="AU78:AV78"/>
+    <mergeCell ref="AU79:AV79"/>
+    <mergeCell ref="AU80:AV80"/>
+    <mergeCell ref="AU111:AV111"/>
+    <mergeCell ref="AU90:AW90"/>
   </mergeCells>
   <conditionalFormatting sqref="T5:V16">
     <cfRule type="expression" dxfId="133" priority="143">
@@ -27588,7 +27588,7 @@
   <dimension ref="B2:BM59"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="AU30" sqref="AU30:AV30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -27642,101 +27642,101 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:65" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="AU2" s="79" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="90"/>
+      <c r="Y2" s="90"/>
+      <c r="AU2" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="80"/>
-      <c r="AW2" s="80"/>
-      <c r="AX2" s="81"/>
-      <c r="AY2" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="80"/>
-      <c r="BA2" s="81"/>
-      <c r="BB2" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="BC2" s="80"/>
-      <c r="BD2" s="80"/>
-      <c r="BE2" s="80"/>
-      <c r="BF2" s="80"/>
-      <c r="BG2" s="81"/>
-      <c r="BH2" s="79" t="s">
+      <c r="AV2" s="84"/>
+      <c r="AW2" s="84"/>
+      <c r="AX2" s="85"/>
+      <c r="AY2" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="84"/>
+      <c r="BA2" s="85"/>
+      <c r="BB2" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="84"/>
+      <c r="BD2" s="84"/>
+      <c r="BE2" s="84"/>
+      <c r="BF2" s="84"/>
+      <c r="BG2" s="85"/>
+      <c r="BH2" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="BI2" s="80"/>
-      <c r="BJ2" s="81"/>
-      <c r="BK2" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="BL2" s="80"/>
-      <c r="BM2" s="81"/>
+      <c r="BI2" s="84"/>
+      <c r="BJ2" s="85"/>
+      <c r="BK2" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL2" s="84"/>
+      <c r="BM2" s="85"/>
     </row>
     <row r="3" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
       <c r="C3" s="24"/>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
       <c r="G3" s="20"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74" t="s">
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74" t="s">
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74" t="s">
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74" t="s">
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74" t="s">
+      <c r="U3" s="88"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
+      <c r="X3" s="88"/>
+      <c r="Y3" s="88"/>
       <c r="AA3" s="4" t="s">
         <v>59</v>
       </c>
@@ -28895,32 +28895,32 @@
       </c>
     </row>
     <row r="10" spans="2:65" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="76"/>
-      <c r="V10" s="76"/>
-      <c r="W10" s="76"/>
-      <c r="X10" s="76"/>
-      <c r="Y10" s="76"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="90"/>
+      <c r="R10" s="90"/>
+      <c r="S10" s="90"/>
+      <c r="T10" s="90"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="90"/>
+      <c r="W10" s="90"/>
+      <c r="X10" s="90"/>
+      <c r="Y10" s="90"/>
       <c r="AU10" s="31">
         <v>7</v>
       </c>
@@ -28999,42 +28999,42 @@
     <row r="11" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
       <c r="C11" s="24"/>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="74" t="s">
+      <c r="H11" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74" t="s">
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74" t="s">
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74" t="s">
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74" t="s">
+      <c r="R11" s="88"/>
+      <c r="S11" s="88"/>
+      <c r="T11" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U11" s="74"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="74" t="s">
+      <c r="U11" s="88"/>
+      <c r="V11" s="88"/>
+      <c r="W11" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X11" s="74"/>
-      <c r="Y11" s="74"/>
+      <c r="X11" s="88"/>
+      <c r="Y11" s="88"/>
       <c r="AA11" s="4" t="s">
         <v>59</v>
       </c>
@@ -29175,30 +29175,46 @@
         <f>IF(AB4=0,"Vencedor Q1",AB4)</f>
         <v>Brasil</v>
       </c>
-      <c r="D12" s="56"/>
+      <c r="D12" s="56">
+        <v>0</v>
+      </c>
       <c r="E12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="34">
+        <v>3</v>
+      </c>
       <c r="G12" s="21" t="str">
         <f>IF(AB7=0,"Vencedor Q4",AB7)</f>
         <v>Polônia</v>
       </c>
-      <c r="H12" s="33"/>
+      <c r="H12" s="33">
+        <v>26</v>
+      </c>
       <c r="I12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="34"/>
-      <c r="K12" s="33"/>
+      <c r="J12" s="34">
+        <v>28</v>
+      </c>
+      <c r="K12" s="33">
+        <v>19</v>
+      </c>
       <c r="L12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="34"/>
-      <c r="N12" s="33"/>
+      <c r="M12" s="34">
+        <v>25</v>
+      </c>
+      <c r="N12" s="33">
+        <v>21</v>
+      </c>
       <c r="O12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P12" s="34"/>
+      <c r="P12" s="34">
+        <v>25</v>
+      </c>
       <c r="Q12" s="33"/>
       <c r="R12" s="11" t="s">
         <v>63</v>
@@ -29211,30 +29227,30 @@
       <c r="V12" s="34"/>
       <c r="W12" s="12">
         <f>SUM(H12,K12,N12,Q12,T12)</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="X12" s="13" t="s">
         <v>63</v>
       </c>
       <c r="Y12" s="14">
         <f>SUM(J12,M12,P12,S12,V12)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AA12" s="4">
         <f>AD12+AE12</f>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="4" t="str">
         <f>IF(OR(D12="",F12=""),0,IF(D12&gt;F12,C12,G12))</f>
-        <v>0</v>
+        <v>Polônia</v>
       </c>
       <c r="AC12" s="4">
         <f>IF(OR(D12="",F12=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="4">
         <f>IF(OR(D12="",F12=""),0,IF(D12&gt;F12,D12,F12))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE12" s="4">
         <f>IF(OR(D12="",F12=""),0,IF(D12&gt;F12,F12,D12))</f>
@@ -29242,7 +29258,7 @@
       </c>
       <c r="AF12" s="4">
         <f>IF(AND(AD12=3,AE12=0),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" s="4">
         <f>IF(AND(AD12=3,AE12=1),1,0)</f>
@@ -29254,19 +29270,19 @@
       </c>
       <c r="AI12" s="4">
         <f>IF(D12&gt;F12,SUM(H12,K12,N12,Q12,T12,),SUM(J12,M12,P12,S12,V12))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AJ12" s="4">
         <f>IF(D12&gt;F12,SUM(J12,M12,P12,S12,V12),SUM(H12,K12,N12,Q12,T12))</f>
-        <v>0</v>
-      </c>
-      <c r="AL12" s="4">
+        <v>66</v>
+      </c>
+      <c r="AL12" s="4" t="str">
         <f>IF(OR(D12="",F12=""),0,IF(D12&lt;F12,C12,G12))</f>
-        <v>0</v>
+        <v>Brasil</v>
       </c>
       <c r="AM12" s="4">
         <f>IF(OR(D12="",F12=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN12" s="4">
         <f>IF(OR(D12="",F12=""),0,IF(D12&lt;F12,D12,F12))</f>
@@ -29274,7 +29290,7 @@
       </c>
       <c r="AO12" s="4">
         <f>IF(OR(D12="",F12=""),0,IF(D12&lt;F12,F12,D12))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP12" s="4">
         <f>IF(AND(AN12=2,AO12=3),1,0)</f>
@@ -29286,15 +29302,15 @@
       </c>
       <c r="AR12" s="4">
         <f>IF(AND(AN12=0,AO12=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS12" s="4">
         <f>IF(D12&lt;F12,SUM(H12,K12,N12,Q12,T12,),SUM(J12,M12,P12,S12,V12))</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AT12" s="4">
         <f>IF(D12&lt;F12,SUM(J12,M12,P12,S12,V12),SUM(H12,K12,N12,Q12,T12))</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AU12" s="31">
         <v>9</v>
@@ -29379,35 +29395,55 @@
         <f>IF(AB5=0,"Vencedor Q2",AB5)</f>
         <v>Itália</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="56">
+        <v>3</v>
+      </c>
       <c r="E13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="34">
+        <v>1</v>
+      </c>
       <c r="G13" s="21" t="str">
         <f>IF(AB6=0,"Vencedor Q3",AB6)</f>
         <v>Eslovênia</v>
       </c>
-      <c r="H13" s="33"/>
+      <c r="H13" s="33">
+        <v>25</v>
+      </c>
       <c r="I13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="34"/>
-      <c r="K13" s="33"/>
+      <c r="J13" s="34">
+        <v>22</v>
+      </c>
+      <c r="K13" s="33">
+        <v>22</v>
+      </c>
       <c r="L13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="M13" s="34"/>
-      <c r="N13" s="33"/>
+      <c r="M13" s="34">
+        <v>25</v>
+      </c>
+      <c r="N13" s="33">
+        <v>25</v>
+      </c>
       <c r="O13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="33"/>
+      <c r="P13" s="34">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="33">
+        <v>25</v>
+      </c>
       <c r="R13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="S13" s="34"/>
+      <c r="S13" s="34">
+        <v>18</v>
+      </c>
       <c r="T13" s="33"/>
       <c r="U13" s="11" t="s">
         <v>63</v>
@@ -29415,34 +29451,34 @@
       <c r="V13" s="34"/>
       <c r="W13" s="12">
         <f>SUM(H13,K13,N13,Q13,T13)</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="X13" s="13" t="s">
         <v>63</v>
       </c>
       <c r="Y13" s="14">
         <f>SUM(J13,M13,P13,S13,V13)</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="AA13" s="4">
         <f>AD13+AE13</f>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="4" t="str">
         <f>IF(OR(D13="",F13=""),0,IF(D13&gt;F13,C13,G13))</f>
-        <v>0</v>
+        <v>Itália</v>
       </c>
       <c r="AC13" s="4">
         <f>IF(OR(D13="",F13=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13" s="4">
         <f>IF(OR(D13="",F13=""),0,IF(D13&gt;F13,D13,F13))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE13" s="4">
         <f>IF(OR(D13="",F13=""),0,IF(D13&gt;F13,F13,D13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF13" s="4">
         <f>IF(AND(AD13=3,AE13=0),1,0)</f>
@@ -29450,7 +29486,7 @@
       </c>
       <c r="AG13" s="4">
         <f>IF(AND(AD13=3,AE13=1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH13" s="4">
         <f>IF(AND(AD13=3,AE13=2),1,0)</f>
@@ -29458,27 +29494,27 @@
       </c>
       <c r="AI13" s="4">
         <f>IF(D13&gt;F13,SUM(H13,K13,N13,Q13,T13,),SUM(J13,M13,P13,S13,V13))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AJ13" s="4">
         <f>IF(D13&gt;F13,SUM(J13,M13,P13,S13,V13),SUM(H13,K13,N13,Q13,T13))</f>
-        <v>0</v>
-      </c>
-      <c r="AL13" s="4">
+        <v>86</v>
+      </c>
+      <c r="AL13" s="4" t="str">
         <f>IF(OR(D13="",F13=""),0,IF(D13&lt;F13,C13,G13))</f>
-        <v>0</v>
+        <v>Eslovênia</v>
       </c>
       <c r="AM13" s="4">
         <f>IF(OR(D13="",F13=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN13" s="4">
         <f>IF(OR(D13="",F13=""),0,IF(D13&lt;F13,D13,F13))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO13" s="4">
         <f>IF(OR(D13="",F13=""),0,IF(D13&lt;F13,F13,D13))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP13" s="4">
         <f>IF(AND(AN13=2,AO13=3),1,0)</f>
@@ -29486,7 +29522,7 @@
       </c>
       <c r="AQ13" s="4">
         <f>IF(AND(AN13=1,AO13=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR13" s="4">
         <f>IF(AND(AN13=0,AO13=3),1,0)</f>
@@ -29494,11 +29530,11 @@
       </c>
       <c r="AS13" s="4">
         <f>IF(D13&lt;F13,SUM(H13,K13,N13,Q13,T13,),SUM(J13,M13,P13,S13,V13))</f>
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="AT13" s="4">
         <f>IF(D13&lt;F13,SUM(J13,M13,P13,S13,V13),SUM(H13,K13,N13,Q13,T13))</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AU13" s="31">
         <v>10</v>
@@ -29804,32 +29840,32 @@
       </c>
     </row>
     <row r="17" spans="2:65" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="90"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="90"/>
       <c r="AA17" s="4" t="s">
         <v>59</v>
       </c>
@@ -29965,61 +30001,61 @@
     <row r="18" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="78" t="s">
+      <c r="D18" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="74" t="s">
+      <c r="H18" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74" t="s">
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="74" t="s">
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74" t="s">
+      <c r="O18" s="88"/>
+      <c r="P18" s="88"/>
+      <c r="Q18" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R18" s="74"/>
-      <c r="S18" s="74"/>
-      <c r="T18" s="74" t="s">
+      <c r="R18" s="88"/>
+      <c r="S18" s="88"/>
+      <c r="T18" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74" t="s">
+      <c r="U18" s="88"/>
+      <c r="V18" s="88"/>
+      <c r="W18" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X18" s="74"/>
-      <c r="Y18" s="74"/>
+      <c r="X18" s="88"/>
+      <c r="Y18" s="88"/>
       <c r="AA18" s="4">
         <f>AD18+AE18</f>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB18" s="4" t="str">
         <f>IF(OR(D19="",F19=""),0,IF(D19&gt;F19,C19,G19))</f>
-        <v>0</v>
+        <v>Brasil</v>
       </c>
       <c r="AC18" s="4">
         <f>IF(OR(D19="",F19=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD18" s="4">
         <f>IF(OR(D19="",F19=""),0,IF(D19&gt;F19,D19,F19))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE18" s="4">
         <f>IF(OR(D19="",F19=""),0,IF(D19&gt;F19,F19,D19))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" s="4">
         <f>IF(AND(AD18=3,AE18=0),1,0)</f>
@@ -30027,7 +30063,7 @@
       </c>
       <c r="AG18" s="4">
         <f>IF(AND(AD18=3,AE18=1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH18" s="4">
         <f>IF(AND(AD18=3,AE18=2),1,0)</f>
@@ -30035,27 +30071,27 @@
       </c>
       <c r="AI18" s="4">
         <f>IF(D19&gt;F19,SUM(H19,K19,N19,Q19,T19,),SUM(J19,M19,P19,S19,V19))</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="AJ18" s="4">
         <f>IF(D19&gt;F19,SUM(J19,M19,P19,S19,V19),SUM(H19,K19,N19,Q19,T19))</f>
-        <v>0</v>
-      </c>
-      <c r="AL18" s="4">
+        <v>87</v>
+      </c>
+      <c r="AL18" s="4" t="str">
         <f>IF(OR(D19="",F19=""),0,IF(D19&lt;F19,C19,G19))</f>
-        <v>0</v>
+        <v>Eslovênia</v>
       </c>
       <c r="AM18" s="4">
         <f>IF(OR(D19="",F19=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="4">
         <f>IF(OR(D19="",F19=""),0,IF(D19&lt;F19,D19,F19))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO18" s="4">
         <f>IF(OR(D19="",F19=""),0,IF(D19&lt;F19,F19,D19))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP18" s="4">
         <f>IF(AND(AN18=2,AO18=3),1,0)</f>
@@ -30063,7 +30099,7 @@
       </c>
       <c r="AQ18" s="4">
         <f>IF(AND(AN18=1,AO18=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR18" s="4">
         <f>IF(AND(AN18=0,AO18=3),1,0)</f>
@@ -30071,11 +30107,11 @@
       </c>
       <c r="AS18" s="4">
         <f>IF(D19&lt;F19,SUM(H19,K19,N19,Q19,T19,),SUM(J19,M19,P19,S19,V19))</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="AT18" s="4">
         <f>IF(D19&lt;F19,SUM(J19,M19,P19,S19,V19),SUM(H19,K19,N19,Q19,T19))</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="AU18" s="31">
         <v>15</v>
@@ -30158,37 +30194,57 @@
       </c>
       <c r="C19" s="25" t="str">
         <f>IF(AL12=0,"Perdedor S1",AL12)</f>
-        <v>Perdedor S1</v>
-      </c>
-      <c r="D19" s="56"/>
+        <v>Brasil</v>
+      </c>
+      <c r="D19" s="56">
+        <v>3</v>
+      </c>
       <c r="E19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="34"/>
+      <c r="F19" s="34">
+        <v>1</v>
+      </c>
       <c r="G19" s="21" t="str">
         <f>IF(AL13=0,"Perdedor S2",AL13)</f>
-        <v>Perdedor S2</v>
-      </c>
-      <c r="H19" s="33"/>
+        <v>Eslovênia</v>
+      </c>
+      <c r="H19" s="33">
+        <v>23</v>
+      </c>
       <c r="I19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="33"/>
+      <c r="J19" s="34">
+        <v>25</v>
+      </c>
+      <c r="K19" s="33">
+        <v>25</v>
+      </c>
       <c r="L19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="34"/>
-      <c r="N19" s="33"/>
+      <c r="M19" s="34">
+        <v>20</v>
+      </c>
+      <c r="N19" s="33">
+        <v>25</v>
+      </c>
       <c r="O19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="33"/>
+      <c r="P19" s="34">
+        <v>23</v>
+      </c>
+      <c r="Q19" s="33">
+        <v>25</v>
+      </c>
       <c r="R19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="34"/>
+      <c r="S19" s="34">
+        <v>19</v>
+      </c>
       <c r="T19" s="33"/>
       <c r="U19" s="11" t="s">
         <v>63</v>
@@ -30196,14 +30252,14 @@
       <c r="V19" s="34"/>
       <c r="W19" s="12">
         <f>SUM(H19,K19,N19,Q19,T19)</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>63</v>
       </c>
       <c r="Y19" s="14">
         <f>SUM(J19,M19,P19,S19,V19)</f>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="AU19" s="31">
         <v>16</v>
@@ -30439,32 +30495,32 @@
       </c>
     </row>
     <row r="23" spans="2:65" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="76"/>
-      <c r="O23" s="76"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="76"/>
-      <c r="S23" s="76"/>
-      <c r="T23" s="76"/>
-      <c r="U23" s="76"/>
-      <c r="V23" s="76"/>
-      <c r="W23" s="76"/>
-      <c r="X23" s="76"/>
-      <c r="Y23" s="76"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="90"/>
+      <c r="O23" s="90"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="90"/>
+      <c r="R23" s="90"/>
+      <c r="S23" s="90"/>
+      <c r="T23" s="90"/>
+      <c r="U23" s="90"/>
+      <c r="V23" s="90"/>
+      <c r="W23" s="90"/>
+      <c r="X23" s="90"/>
+      <c r="Y23" s="90"/>
       <c r="AA23" s="4" t="s">
         <v>59</v>
       </c>
@@ -30531,57 +30587,57 @@
     <row r="24" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="78" t="s">
+      <c r="D24" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
       <c r="G24" s="20"/>
-      <c r="H24" s="74" t="s">
+      <c r="H24" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74" t="s">
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="L24" s="74"/>
-      <c r="M24" s="74"/>
-      <c r="N24" s="74" t="s">
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O24" s="74"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="74" t="s">
+      <c r="O24" s="88"/>
+      <c r="P24" s="88"/>
+      <c r="Q24" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="R24" s="74"/>
-      <c r="S24" s="74"/>
-      <c r="T24" s="74" t="s">
+      <c r="R24" s="88"/>
+      <c r="S24" s="88"/>
+      <c r="T24" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="U24" s="74"/>
-      <c r="V24" s="74"/>
-      <c r="W24" s="74" t="s">
+      <c r="U24" s="88"/>
+      <c r="V24" s="88"/>
+      <c r="W24" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="X24" s="74"/>
-      <c r="Y24" s="74"/>
+      <c r="X24" s="88"/>
+      <c r="Y24" s="88"/>
       <c r="AA24" s="4">
         <f>AD24+AE24</f>
-        <v>0</v>
-      </c>
-      <c r="AB24" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="4" t="str">
         <f>IF(OR(D25="",F25=""),0,IF(D25&gt;F25,C25,G25))</f>
-        <v>0</v>
+        <v>Polônia</v>
       </c>
       <c r="AC24" s="4">
         <f>IF(OR(D25="",F25=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD24" s="4">
         <f>IF(OR(D25="",F25=""),0,IF(D25&gt;F25,D25,F25))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE24" s="4">
         <f>IF(OR(D25="",F25=""),0,IF(D25&gt;F25,F25,D25))</f>
@@ -30589,7 +30645,7 @@
       </c>
       <c r="AF24" s="4">
         <f>IF(AND(AD24=3,AE24=0),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG24" s="4">
         <f>IF(AND(AD24=3,AE24=1),1,0)</f>
@@ -30601,19 +30657,19 @@
       </c>
       <c r="AI24" s="4">
         <f>IF(D25&gt;F25,SUM(H25,K25,N25,Q25,T25,),SUM(J25,M25,P25,S25,V25))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AJ24" s="4">
         <f>IF(D25&gt;F25,SUM(J25,M25,P25,S25,V25),SUM(H25,K25,N25,Q25,T25))</f>
-        <v>0</v>
-      </c>
-      <c r="AL24" s="4">
+        <v>55</v>
+      </c>
+      <c r="AL24" s="4" t="str">
         <f>IF(OR(D25="",F25=""),0,IF(D25&lt;F25,C25,G25))</f>
-        <v>0</v>
+        <v>Itália</v>
       </c>
       <c r="AM24" s="4">
         <f>IF(OR(D25="",F25=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN24" s="4">
         <f>IF(OR(D25="",F25=""),0,IF(D25&lt;F25,D25,F25))</f>
@@ -30621,7 +30677,7 @@
       </c>
       <c r="AO24" s="4">
         <f>IF(OR(D25="",F25=""),0,IF(D25&lt;F25,F25,D25))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP24" s="4">
         <f>IF(AND(AN24=2,AO24=3),1,0)</f>
@@ -30633,15 +30689,15 @@
       </c>
       <c r="AR24" s="4">
         <f>IF(AND(AN24=0,AO24=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS24" s="4">
         <f>IF(D25&lt;F25,SUM(H25,K25,N25,Q25,T25,),SUM(J25,M25,P25,S25,V25))</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="AT24" s="4">
         <f>IF(D25&lt;F25,SUM(J25,M25,P25,S25,V25),SUM(H25,K25,N25,Q25,T25))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AU24" s="54"/>
       <c r="AV24" s="7" t="s">
@@ -30655,32 +30711,48 @@
       </c>
       <c r="C25" s="25" t="str">
         <f>IF(AB12=0,"Vencedor S1",AB12)</f>
-        <v>Vencedor S1</v>
-      </c>
-      <c r="D25" s="56"/>
+        <v>Polônia</v>
+      </c>
+      <c r="D25" s="56">
+        <v>3</v>
+      </c>
       <c r="E25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="34"/>
+      <c r="F25" s="34">
+        <v>0</v>
+      </c>
       <c r="G25" s="21" t="str">
         <f>IF(AB13=0,"Vencedor S2",AB13)</f>
-        <v>Vencedor S2</v>
-      </c>
-      <c r="H25" s="33"/>
+        <v>Itália</v>
+      </c>
+      <c r="H25" s="33">
+        <v>25</v>
+      </c>
       <c r="I25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="33"/>
+      <c r="J25" s="34">
+        <v>22</v>
+      </c>
+      <c r="K25" s="33">
+        <v>25</v>
+      </c>
       <c r="L25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="M25" s="34"/>
-      <c r="N25" s="33"/>
+      <c r="M25" s="34">
+        <v>19</v>
+      </c>
+      <c r="N25" s="33">
+        <v>25</v>
+      </c>
       <c r="O25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P25" s="34"/>
+      <c r="P25" s="34">
+        <v>14</v>
+      </c>
       <c r="Q25" s="33"/>
       <c r="R25" s="11" t="s">
         <v>63</v>
@@ -30693,14 +30765,14 @@
       <c r="V25" s="34"/>
       <c r="W25" s="12">
         <f>SUM(H25,K25,N25,Q25,T25)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X25" s="13" t="s">
         <v>63</v>
       </c>
       <c r="Y25" s="14">
         <f>SUM(J25,M25,P25,S25,V25)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="AU25" s="55"/>
       <c r="AV25" s="7" t="s">
@@ -30768,10 +30840,10 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
       <c r="Y28" s="39"/>
-      <c r="AU28" s="83" t="s">
+      <c r="AU28" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="AV28" s="84"/>
+      <c r="AV28" s="79"/>
       <c r="AW28" s="64"/>
     </row>
     <row r="29" spans="2:65" s="41" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -30780,15 +30852,15 @@
       </c>
       <c r="C29" s="48" t="str">
         <f>IF(AB24=0,"Campeão",AB24)</f>
-        <v>Campeão</v>
+        <v>Polônia</v>
       </c>
       <c r="D29" s="45"/>
       <c r="F29" s="47"/>
       <c r="G29" s="42"/>
-      <c r="AU29" s="89" t="s">
+      <c r="AU29" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="AV29" s="90"/>
+      <c r="AV29" s="81"/>
       <c r="AW29" s="65"/>
     </row>
     <row r="30" spans="2:65" s="41" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -30797,15 +30869,15 @@
       </c>
       <c r="C30" s="49" t="str">
         <f>IF(AL24=0,"Vice",AL24)</f>
-        <v>Vice</v>
+        <v>Itália</v>
       </c>
       <c r="D30" s="45"/>
       <c r="F30" s="47"/>
       <c r="G30" s="42"/>
-      <c r="AU30" s="85" t="s">
+      <c r="AU30" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="AV30" s="86"/>
+      <c r="AV30" s="75"/>
       <c r="AW30" s="66"/>
     </row>
     <row r="31" spans="2:65" ht="24.75" x14ac:dyDescent="0.25">
@@ -30814,7 +30886,7 @@
       </c>
       <c r="C31" s="49" t="str">
         <f>IF(AB18=0,"Terceiro",AB18)</f>
-        <v>Terceiro</v>
+        <v>Brasil</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="41"/>
@@ -30838,10 +30910,10 @@
       <c r="W31" s="41"/>
       <c r="X31" s="41"/>
       <c r="Y31" s="41"/>
-      <c r="AU31" s="85" t="s">
+      <c r="AU31" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="AV31" s="86"/>
+      <c r="AV31" s="75"/>
       <c r="AW31" s="66"/>
     </row>
     <row r="32" spans="2:65" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -30850,12 +30922,12 @@
       </c>
       <c r="C32" s="59" t="str">
         <f>IF(AL18=0,"",AL18)</f>
-        <v/>
-      </c>
-      <c r="AU32" s="85" t="s">
+        <v>Eslovênia</v>
+      </c>
+      <c r="AU32" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="AV32" s="86"/>
+      <c r="AV32" s="75"/>
       <c r="AW32" s="66"/>
     </row>
     <row r="33" spans="2:49" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -30866,10 +30938,10 @@
         <f>IFERROR(VLOOKUP(SMALL($AK$34:$AK$37,1),$AK$34:$AL$37,2,FALSE),"")</f>
         <v>França</v>
       </c>
-      <c r="AU33" s="87" t="s">
+      <c r="AU33" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="AV33" s="88"/>
+      <c r="AV33" s="77"/>
       <c r="AW33" s="67"/>
     </row>
     <row r="34" spans="2:49" x14ac:dyDescent="0.25">
@@ -31241,22 +31313,23 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="45">
-    <mergeCell ref="AU29:AV29"/>
-    <mergeCell ref="AU30:AV30"/>
-    <mergeCell ref="AU31:AV31"/>
-    <mergeCell ref="AU32:AV32"/>
-    <mergeCell ref="AU33:AV33"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="AU23:AV23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="B23:Y23"/>
-    <mergeCell ref="AU28:AV28"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B10:Y10"/>
+    <mergeCell ref="B17:Y17"/>
+    <mergeCell ref="B2:Y2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AY2:BA2"/>
+    <mergeCell ref="BB2:BG2"/>
+    <mergeCell ref="BH2:BJ2"/>
+    <mergeCell ref="BK2:BM2"/>
     <mergeCell ref="T18:V18"/>
     <mergeCell ref="W18:Y18"/>
     <mergeCell ref="D11:F11"/>
@@ -31269,23 +31342,22 @@
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AY2:BA2"/>
-    <mergeCell ref="BB2:BG2"/>
-    <mergeCell ref="BH2:BJ2"/>
-    <mergeCell ref="BK2:BM2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B10:Y10"/>
-    <mergeCell ref="B17:Y17"/>
-    <mergeCell ref="B2:Y2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="AU23:AV23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="B23:Y23"/>
+    <mergeCell ref="AU28:AV28"/>
+    <mergeCell ref="AU29:AV29"/>
+    <mergeCell ref="AU30:AV30"/>
+    <mergeCell ref="AU31:AV31"/>
+    <mergeCell ref="AU32:AV32"/>
+    <mergeCell ref="AU33:AV33"/>
   </mergeCells>
   <conditionalFormatting sqref="T4:V7 T12:V13">
     <cfRule type="expression" dxfId="25" priority="82">
@@ -31461,6 +31533,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -31693,24 +31782,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1A4F3B6-8EF3-43FC-AA6E-56F4B11E76F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31727,22 +31817,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>